<commit_message>
Aggiunta ETP + Aggiornamento Packet Tracer
</commit_message>
<xml_diff>
--- a/Matematica/Italia 19 maggio.xlsx
+++ b/Matematica/Italia 19 maggio.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="137">
   <si>
     <t>Giorno_Cont</t>
   </si>
@@ -383,6 +383,48 @@
   </si>
   <si>
     <t>5/18/20</t>
+  </si>
+  <si>
+    <t>5/19/20</t>
+  </si>
+  <si>
+    <t>5/20/20</t>
+  </si>
+  <si>
+    <t>5/21/20</t>
+  </si>
+  <si>
+    <t>5/22/20</t>
+  </si>
+  <si>
+    <t>5/23/20</t>
+  </si>
+  <si>
+    <t>5/24/20</t>
+  </si>
+  <si>
+    <t>5/25/20</t>
+  </si>
+  <si>
+    <t>5/26/20</t>
+  </si>
+  <si>
+    <t>5/27/20</t>
+  </si>
+  <si>
+    <t>5/28/20</t>
+  </si>
+  <si>
+    <t>5/29/20</t>
+  </si>
+  <si>
+    <t>5/30/20</t>
+  </si>
+  <si>
+    <t>5/31/20</t>
+  </si>
+  <si>
+    <t>6/1/20</t>
   </si>
 </sst>
 </file>
@@ -714,7 +756,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E119"/>
+  <dimension ref="A1:E133"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1595,10 +1637,10 @@
         <v>55</v>
       </c>
       <c r="C52">
-        <v>12462</v>
+        <v>15113</v>
       </c>
       <c r="D52">
-        <v>827</v>
+        <v>1016</v>
       </c>
       <c r="E52">
         <v>1045</v>
@@ -2741,6 +2783,244 @@
       </c>
       <c r="E119">
         <v>127326</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5">
+      <c r="A120">
+        <v>118</v>
+      </c>
+      <c r="B120" t="s">
+        <v>123</v>
+      </c>
+      <c r="C120">
+        <v>226699</v>
+      </c>
+      <c r="D120">
+        <v>32169</v>
+      </c>
+      <c r="E120">
+        <v>129401</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5">
+      <c r="A121">
+        <v>119</v>
+      </c>
+      <c r="B121" t="s">
+        <v>124</v>
+      </c>
+      <c r="C121">
+        <v>227364</v>
+      </c>
+      <c r="D121">
+        <v>32330</v>
+      </c>
+      <c r="E121">
+        <v>132282</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5">
+      <c r="A122">
+        <v>120</v>
+      </c>
+      <c r="B122" t="s">
+        <v>125</v>
+      </c>
+      <c r="C122">
+        <v>228006</v>
+      </c>
+      <c r="D122">
+        <v>32486</v>
+      </c>
+      <c r="E122">
+        <v>134560</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5">
+      <c r="A123">
+        <v>121</v>
+      </c>
+      <c r="B123" t="s">
+        <v>126</v>
+      </c>
+      <c r="C123">
+        <v>228658</v>
+      </c>
+      <c r="D123">
+        <v>32616</v>
+      </c>
+      <c r="E123">
+        <v>136720</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5">
+      <c r="A124">
+        <v>122</v>
+      </c>
+      <c r="B124" t="s">
+        <v>127</v>
+      </c>
+      <c r="C124">
+        <v>229327</v>
+      </c>
+      <c r="D124">
+        <v>32735</v>
+      </c>
+      <c r="E124">
+        <v>138840</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5">
+      <c r="A125">
+        <v>123</v>
+      </c>
+      <c r="B125" t="s">
+        <v>128</v>
+      </c>
+      <c r="C125">
+        <v>229858</v>
+      </c>
+      <c r="D125">
+        <v>32785</v>
+      </c>
+      <c r="E125">
+        <v>140479</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5">
+      <c r="A126">
+        <v>124</v>
+      </c>
+      <c r="B126" t="s">
+        <v>129</v>
+      </c>
+      <c r="C126">
+        <v>230158</v>
+      </c>
+      <c r="D126">
+        <v>32877</v>
+      </c>
+      <c r="E126">
+        <v>141981</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5">
+      <c r="A127">
+        <v>125</v>
+      </c>
+      <c r="B127" t="s">
+        <v>130</v>
+      </c>
+      <c r="C127">
+        <v>230555</v>
+      </c>
+      <c r="D127">
+        <v>32955</v>
+      </c>
+      <c r="E127">
+        <v>144658</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5">
+      <c r="A128">
+        <v>126</v>
+      </c>
+      <c r="B128" t="s">
+        <v>131</v>
+      </c>
+      <c r="C128">
+        <v>231139</v>
+      </c>
+      <c r="D128">
+        <v>33072</v>
+      </c>
+      <c r="E128">
+        <v>147101</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5">
+      <c r="A129">
+        <v>127</v>
+      </c>
+      <c r="B129" t="s">
+        <v>132</v>
+      </c>
+      <c r="C129">
+        <v>231732</v>
+      </c>
+      <c r="D129">
+        <v>33142</v>
+      </c>
+      <c r="E129">
+        <v>150604</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5">
+      <c r="A130">
+        <v>128</v>
+      </c>
+      <c r="B130" t="s">
+        <v>133</v>
+      </c>
+      <c r="C130">
+        <v>232248</v>
+      </c>
+      <c r="D130">
+        <v>33229</v>
+      </c>
+      <c r="E130">
+        <v>152844</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5">
+      <c r="A131">
+        <v>129</v>
+      </c>
+      <c r="B131" t="s">
+        <v>134</v>
+      </c>
+      <c r="C131">
+        <v>232664</v>
+      </c>
+      <c r="D131">
+        <v>33340</v>
+      </c>
+      <c r="E131">
+        <v>155633</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5">
+      <c r="A132">
+        <v>130</v>
+      </c>
+      <c r="B132" t="s">
+        <v>135</v>
+      </c>
+      <c r="C132">
+        <v>232997</v>
+      </c>
+      <c r="D132">
+        <v>33415</v>
+      </c>
+      <c r="E132">
+        <v>157507</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5">
+      <c r="A133">
+        <v>131</v>
+      </c>
+      <c r="B133" t="s">
+        <v>136</v>
+      </c>
+      <c r="C133">
+        <v>233197</v>
+      </c>
+      <c r="D133">
+        <v>33475</v>
+      </c>
+      <c r="E133">
+        <v>158355</v>
       </c>
     </row>
   </sheetData>

</xml_diff>